<commit_message>
Eval: Added dangling data and updates for evaluations
</commit_message>
<xml_diff>
--- a/eval/e52/observations.xlsx
+++ b/eval/e52/observations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="7680" yWindow="0" windowWidth="25600" windowHeight="25060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -166,6 +166,27 @@
   </si>
   <si>
     <t>What happens when there's an error in the first version of the code that the user produces?</t>
+  </si>
+  <si>
+    <t>Jeremy Faludi</t>
+  </si>
+  <si>
+    <t>HTML</t>
+  </si>
+  <si>
+    <t>6 mo-1 year overall</t>
+  </si>
+  <si>
+    <t>Once every 10 years</t>
+  </si>
+  <si>
+    <t>Daniel Seita</t>
+  </si>
+  <si>
+    <t>Christine Gregg</t>
+  </si>
+  <si>
+    <t>MATLAB</t>
   </si>
 </sst>
 </file>
@@ -214,8 +235,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -226,13 +249,15 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -565,7 +590,7 @@
   <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -900,6 +925,54 @@
         <v>48</v>
       </c>
     </row>
+    <row r="7" spans="1:21">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M9" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="18" spans="11:13">
       <c r="K18" t="s">
         <v>39</v>

</xml_diff>